<commit_message>
Moved the Logic for Buildingsanity to the Scenario folders
</commit_message>
<xml_diff>
--- a/docs/Logic Requirements/Ageipelago Attila the Hun.xlsx
+++ b/docs/Logic Requirements/Ageipelago Attila the Hun.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\stefb\OneDrive\Desktop\Logic Requirements\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{49723FAC-1A4C-492A-8478-2080EE0A6E88}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C81CCDE2-4BC5-48F1-A5CC-86BCDF63FFDF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-28920" yWindow="-120" windowWidth="29040" windowHeight="15720" firstSheet="1" activeTab="6" xr2:uid="{B80992DC-780F-4856-A6B0-D26FA95FCBC0}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" tabRatio="639" activeTab="6" xr2:uid="{B80992DC-780F-4856-A6B0-D26FA95FCBC0}"/>
   </bookViews>
   <sheets>
     <sheet name="Attila the Hun" sheetId="1" r:id="rId1"/>
@@ -43,7 +43,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="266" uniqueCount="170">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="355" uniqueCount="183">
   <si>
     <t>Scenario</t>
   </si>
@@ -4532,11 +4532,6 @@
 - Purple Villagers</t>
   </si>
   <si>
-    <t>Requires
-- Purple Villagers
-+Town Center Wood/Stone</t>
-  </si>
-  <si>
     <t>Standard:
 No items required
 Moderate/Hard:
@@ -4544,78 +4539,184 @@
 - Purple Villagers</t>
   </si>
   <si>
+    <t>DefeatBurgundyAll</t>
+  </si>
+  <si>
+    <t>DefeatMetz</t>
+  </si>
+  <si>
+    <t>DefeatOrléans</t>
+  </si>
+  <si>
+    <t>DefeatRomanArmy</t>
+  </si>
+  <si>
+    <t>TributeBurgundyAll</t>
+  </si>
+  <si>
+    <t>CastleBurgundyAll</t>
+  </si>
+  <si>
+    <t>DefeatOrAllyBurgundyAny</t>
+  </si>
+  <si>
+    <t>Requires
+-Town Center Wood/Stone</t>
+  </si>
+  <si>
+    <t>DefeatAlans</t>
+  </si>
+  <si>
+    <t>DefeatVisigoths</t>
+  </si>
+  <si>
+    <t>DefeatRomans</t>
+  </si>
+  <si>
+    <t>DefeatPatavium</t>
+  </si>
+  <si>
+    <t>DefeatMediolanum</t>
+  </si>
+  <si>
+    <t>DefeatAquileia</t>
+  </si>
+  <si>
+    <t>DefeatVerona</t>
+  </si>
+  <si>
+    <t>DefeatTheItalian</t>
+  </si>
+  <si>
+    <t>MeetThePope</t>
+  </si>
+  <si>
+    <t>DestroyPurpleWonder</t>
+  </si>
+  <si>
+    <t>DestroyGreenWonder</t>
+  </si>
+  <si>
+    <t>DestroyRedWonder</t>
+  </si>
+  <si>
+    <t>DestroyOrangeWonder</t>
+  </si>
+  <si>
+    <t>DestroyPurpleWonder2</t>
+  </si>
+  <si>
+    <t>Logic (Buildingsanity)</t>
+  </si>
+  <si>
     <t>Requires EITHER
 - Bleda's Base
 OR
 - Attilla's Base
-+Town Center Wood/Stone</t>
-  </si>
-  <si>
-    <t>DefeatBurgundyAll</t>
-  </si>
-  <si>
-    <t>DefeatMetz</t>
-  </si>
-  <si>
-    <t>DefeatOrléans</t>
-  </si>
-  <si>
-    <t>DefeatRomanArmy</t>
-  </si>
-  <si>
-    <t>TributeBurgundyAll</t>
-  </si>
-  <si>
-    <t>CastleBurgundyAll</t>
-  </si>
-  <si>
-    <t>DefeatOrAllyBurgundyAny</t>
++ Town Center Wood/Stone</t>
+  </si>
+  <si>
+    <t>Requires EITHER
+- No Item
+OR
+- Town Center</t>
   </si>
   <si>
     <t>Requires
--Town Center Wood/Stone</t>
-  </si>
-  <si>
-    <t>DefeatAlans</t>
-  </si>
-  <si>
-    <t>DefeatVisigoths</t>
-  </si>
-  <si>
-    <t>DefeatRomans</t>
-  </si>
-  <si>
-    <t>DefeatPatavium</t>
-  </si>
-  <si>
-    <t>DefeatMediolanum</t>
-  </si>
-  <si>
-    <t>DefeatAquileia</t>
-  </si>
-  <si>
-    <t>DefeatVerona</t>
-  </si>
-  <si>
-    <t>DefeatTheItalian</t>
-  </si>
-  <si>
-    <t>MeetThePope</t>
-  </si>
-  <si>
-    <t>DestroyPurpleWonder</t>
-  </si>
-  <si>
-    <t>DestroyGreenWonder</t>
-  </si>
-  <si>
-    <t>DestroyRedWonder</t>
-  </si>
-  <si>
-    <t>DestroyOrangeWonder</t>
-  </si>
-  <si>
-    <t>DestroyPurpleWonder2</t>
+-Dock</t>
+  </si>
+  <si>
+    <t>Requires EITHER
+- Siege Workshop
+OR
+- Dock
+OR
+-Castle
++Mining Camp/Town Center</t>
+  </si>
+  <si>
+    <t>Requires
+-Castle
++Mining Camp/Town Center</t>
+  </si>
+  <si>
+    <t>Requires EITHER
+- Siege Workshop
+OR
+-Castle
++Mining Camp/Town Center</t>
+  </si>
+  <si>
+    <t>Requires
+- Town Center
++ Castle</t>
+  </si>
+  <si>
+    <t>Requires
+- Town Center Wood/Stone</t>
+  </si>
+  <si>
+    <t>Requires
+- Purple Villagers
++ Town Center Wood/Stone</t>
+  </si>
+  <si>
+    <t>Requires EITHER
+(
+- Siege Workshop
+OR
+- Castle
++ Mining Camp/Town Center)
+OR
+(
+- Town Center
++ Siege Workshop
+OR
+- Castle)</t>
+  </si>
+  <si>
+    <t>Standard:
+No items required
+Moderate:
+Requires EITHER
+(
+- Siege Workshop
+OR
+- Castle
++ Mining Camp/Town Center)
+OR
+(
+- Town Center
++ Siege Workshop
+OR
+- Castle)</t>
+  </si>
+  <si>
+    <t>Requires
+- Town Center
++ Market</t>
+  </si>
+  <si>
+    <t>Requires
+- Town Center
++ 1 Non-Siege Military Building
++ Castle
+OR
+- Siege Workshop</t>
+  </si>
+  <si>
+    <t>Standard:
+Requires 1 Non-Siege Military Building
+Moderate/Hard:
+Requires EITHER
+(
+- Siege Workshop
+OR
+- Dock
+OR
+-Castle
++Mining Camp/Town Center)
++ 1 Non-Siege Military Building</t>
   </si>
 </sst>
 </file>
@@ -5279,9 +5380,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4021AD6D-5731-4FBB-BF2F-CE4CC48789B4}">
   <dimension ref="B2:R9"/>
   <sheetViews>
-    <sheetView topLeftCell="A4" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="B3" sqref="B3:C5"/>
-    </sheetView>
+    <sheetView zoomScaleNormal="100" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
@@ -5633,188 +5732,252 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{BEDF25A3-39E5-43BC-AA21-825EC7632C75}">
-  <dimension ref="B1:C23"/>
+  <dimension ref="B1:D23"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B2" sqref="B2:C14"/>
+      <selection activeCell="E17" sqref="E17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="2" max="2" width="35.140625" customWidth="1"/>
     <col min="3" max="3" width="22.7109375" customWidth="1"/>
+    <col min="4" max="4" width="23.85546875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="2:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
-    <row r="2" spans="2:3" ht="24" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="1" spans="2:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
+    <row r="2" spans="2:4" ht="93.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B2" s="2" t="s">
         <v>94</v>
       </c>
       <c r="C2" s="2" t="s">
         <v>43</v>
       </c>
-    </row>
-    <row r="3" spans="2:3" ht="112.5" x14ac:dyDescent="0.25">
+      <c r="D2" s="2" t="s">
+        <v>168</v>
+      </c>
+    </row>
+    <row r="3" spans="2:4" ht="243.75" x14ac:dyDescent="0.25">
       <c r="B3" s="13" t="s">
         <v>95</v>
       </c>
       <c r="C3" s="5" t="s">
-        <v>147</v>
-      </c>
-    </row>
-    <row r="4" spans="2:3" ht="18.75" x14ac:dyDescent="0.25">
+        <v>169</v>
+      </c>
+      <c r="D3" s="5" t="s">
+        <v>178</v>
+      </c>
+    </row>
+    <row r="4" spans="2:4" ht="18.75" x14ac:dyDescent="0.25">
       <c r="B4" s="14" t="s">
         <v>96</v>
       </c>
       <c r="C4" s="8" t="s">
         <v>115</v>
       </c>
-    </row>
-    <row r="5" spans="2:3" ht="18.75" x14ac:dyDescent="0.25">
+      <c r="D4" s="8" t="s">
+        <v>115</v>
+      </c>
+    </row>
+    <row r="5" spans="2:4" ht="18.75" x14ac:dyDescent="0.25">
       <c r="B5" s="14" t="s">
         <v>97</v>
       </c>
       <c r="C5" s="8" t="s">
         <v>115</v>
       </c>
-    </row>
-    <row r="6" spans="2:3" ht="18.75" x14ac:dyDescent="0.25">
+      <c r="D5" s="8" t="s">
+        <v>115</v>
+      </c>
+    </row>
+    <row r="6" spans="2:4" ht="18.75" x14ac:dyDescent="0.25">
       <c r="B6" s="14" t="s">
         <v>98</v>
       </c>
       <c r="C6" s="8" t="s">
         <v>115</v>
       </c>
-    </row>
-    <row r="7" spans="2:3" ht="37.5" x14ac:dyDescent="0.25">
+      <c r="D6" s="8" t="s">
+        <v>115</v>
+      </c>
+    </row>
+    <row r="7" spans="2:4" ht="18.75" x14ac:dyDescent="0.25">
       <c r="B7" s="14" t="s">
         <v>99</v>
       </c>
       <c r="C7" s="8" t="s">
         <v>115</v>
       </c>
-    </row>
-    <row r="8" spans="2:3" ht="18.75" x14ac:dyDescent="0.25">
+      <c r="D7" s="8" t="s">
+        <v>115</v>
+      </c>
+    </row>
+    <row r="8" spans="2:4" ht="18.75" x14ac:dyDescent="0.25">
       <c r="B8" s="14" t="s">
         <v>100</v>
       </c>
       <c r="C8" s="8" t="s">
         <v>115</v>
       </c>
-    </row>
-    <row r="9" spans="2:3" ht="37.5" x14ac:dyDescent="0.25">
+      <c r="D8" s="8" t="s">
+        <v>115</v>
+      </c>
+    </row>
+    <row r="9" spans="2:4" ht="18.75" x14ac:dyDescent="0.25">
       <c r="B9" s="14" t="s">
         <v>101</v>
       </c>
       <c r="C9" s="8" t="s">
         <v>115</v>
       </c>
-    </row>
-    <row r="10" spans="2:3" ht="37.5" x14ac:dyDescent="0.25">
+      <c r="D9" s="8" t="s">
+        <v>115</v>
+      </c>
+    </row>
+    <row r="10" spans="2:4" ht="18.75" x14ac:dyDescent="0.25">
       <c r="B10" s="14" t="s">
         <v>102</v>
       </c>
       <c r="C10" s="8" t="s">
         <v>115</v>
       </c>
-    </row>
-    <row r="11" spans="2:3" ht="37.5" x14ac:dyDescent="0.25">
+      <c r="D10" s="8" t="s">
+        <v>115</v>
+      </c>
+    </row>
+    <row r="11" spans="2:4" ht="18.75" x14ac:dyDescent="0.25">
       <c r="B11" s="14" t="s">
         <v>103</v>
       </c>
       <c r="C11" s="8" t="s">
         <v>115</v>
       </c>
-    </row>
-    <row r="12" spans="2:3" ht="37.5" x14ac:dyDescent="0.25">
+      <c r="D11" s="8" t="s">
+        <v>115</v>
+      </c>
+    </row>
+    <row r="12" spans="2:4" ht="18.75" x14ac:dyDescent="0.25">
       <c r="B12" s="14" t="s">
         <v>104</v>
       </c>
       <c r="C12" s="8" t="s">
         <v>115</v>
       </c>
-    </row>
-    <row r="13" spans="2:3" ht="18.75" x14ac:dyDescent="0.25">
+      <c r="D12" s="8" t="s">
+        <v>115</v>
+      </c>
+    </row>
+    <row r="13" spans="2:4" ht="18.75" x14ac:dyDescent="0.25">
       <c r="B13" s="14" t="s">
         <v>105</v>
       </c>
       <c r="C13" s="8" t="s">
         <v>115</v>
       </c>
-    </row>
-    <row r="14" spans="2:3" ht="18.75" x14ac:dyDescent="0.25">
+      <c r="D13" s="8" t="s">
+        <v>115</v>
+      </c>
+    </row>
+    <row r="14" spans="2:4" ht="18.75" x14ac:dyDescent="0.25">
       <c r="B14" s="14" t="s">
         <v>106</v>
       </c>
       <c r="C14" s="8" t="s">
         <v>115</v>
       </c>
-    </row>
-    <row r="15" spans="2:3" ht="18.75" x14ac:dyDescent="0.25">
+      <c r="D14" s="8" t="s">
+        <v>115</v>
+      </c>
+    </row>
+    <row r="15" spans="2:4" ht="18.75" x14ac:dyDescent="0.25">
       <c r="B15" s="14" t="s">
         <v>107</v>
       </c>
       <c r="C15" s="8" t="s">
         <v>115</v>
       </c>
-    </row>
-    <row r="16" spans="2:3" ht="18.75" x14ac:dyDescent="0.25">
+      <c r="D15" s="8" t="s">
+        <v>115</v>
+      </c>
+    </row>
+    <row r="16" spans="2:4" ht="18.75" x14ac:dyDescent="0.25">
       <c r="B16" s="14" t="s">
         <v>108</v>
       </c>
       <c r="C16" s="8" t="s">
         <v>115</v>
       </c>
-    </row>
-    <row r="17" spans="2:3" ht="112.5" x14ac:dyDescent="0.25">
+      <c r="D16" s="8" t="s">
+        <v>115</v>
+      </c>
+    </row>
+    <row r="17" spans="2:4" ht="112.5" x14ac:dyDescent="0.25">
       <c r="B17" s="14" t="s">
         <v>109</v>
       </c>
       <c r="C17" s="8" t="s">
-        <v>147</v>
-      </c>
-    </row>
-    <row r="18" spans="2:3" ht="112.5" x14ac:dyDescent="0.25">
+        <v>169</v>
+      </c>
+      <c r="D17" s="5" t="s">
+        <v>170</v>
+      </c>
+    </row>
+    <row r="18" spans="2:4" ht="112.5" x14ac:dyDescent="0.25">
       <c r="B18" s="14" t="s">
         <v>110</v>
       </c>
       <c r="C18" s="8" t="s">
         <v>116</v>
       </c>
-    </row>
-    <row r="19" spans="2:3" ht="112.5" x14ac:dyDescent="0.25">
+      <c r="D18" s="8" t="s">
+        <v>115</v>
+      </c>
+    </row>
+    <row r="19" spans="2:4" ht="300" x14ac:dyDescent="0.25">
       <c r="B19" s="14" t="s">
         <v>111</v>
       </c>
       <c r="C19" s="8" t="s">
-        <v>147</v>
-      </c>
-    </row>
-    <row r="20" spans="2:3" ht="112.5" x14ac:dyDescent="0.25">
+        <v>169</v>
+      </c>
+      <c r="D19" s="8" t="s">
+        <v>179</v>
+      </c>
+    </row>
+    <row r="20" spans="2:4" ht="300" x14ac:dyDescent="0.25">
       <c r="B20" s="14" t="s">
         <v>112</v>
       </c>
       <c r="C20" s="8" t="s">
-        <v>147</v>
-      </c>
-    </row>
-    <row r="21" spans="2:3" ht="112.5" x14ac:dyDescent="0.25">
+        <v>169</v>
+      </c>
+      <c r="D20" s="8" t="s">
+        <v>179</v>
+      </c>
+    </row>
+    <row r="21" spans="2:4" ht="243.75" x14ac:dyDescent="0.25">
       <c r="B21" s="14" t="s">
         <v>113</v>
       </c>
       <c r="C21" s="8" t="s">
-        <v>147</v>
-      </c>
-    </row>
-    <row r="22" spans="2:3" ht="112.5" x14ac:dyDescent="0.25">
+        <v>169</v>
+      </c>
+      <c r="D21" s="5" t="s">
+        <v>178</v>
+      </c>
+    </row>
+    <row r="22" spans="2:4" ht="243.75" x14ac:dyDescent="0.25">
       <c r="B22" s="14" t="s">
         <v>114</v>
       </c>
       <c r="C22" s="8" t="s">
-        <v>147</v>
-      </c>
-    </row>
-    <row r="23" spans="2:3" ht="18.75" hidden="1" x14ac:dyDescent="0.25">
+        <v>169</v>
+      </c>
+      <c r="D22" s="5" t="s">
+        <v>178</v>
+      </c>
+    </row>
+    <row r="23" spans="2:4" ht="18.75" hidden="1" x14ac:dyDescent="0.25">
       <c r="B23" s="14"/>
       <c r="C23" s="8"/>
     </row>
@@ -5826,148 +5989,197 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4BC364C8-CB39-4783-9CFD-864E580ACCC1}">
-  <dimension ref="B1:C18"/>
+  <dimension ref="B1:D18"/>
   <sheetViews>
-    <sheetView topLeftCell="A2" workbookViewId="0">
-      <selection activeCell="C15" sqref="C15"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C10" sqref="C10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="2" max="2" width="24.42578125" customWidth="1"/>
-    <col min="3" max="3" width="23" customWidth="1"/>
+    <col min="3" max="4" width="23" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="2:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
-    <row r="2" spans="2:3" ht="47.25" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="1" spans="2:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
+    <row r="2" spans="2:4" ht="70.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B2" s="2" t="s">
         <v>94</v>
       </c>
       <c r="C2" s="2" t="s">
         <v>43</v>
       </c>
-    </row>
-    <row r="3" spans="2:3" ht="37.5" x14ac:dyDescent="0.25">
+      <c r="D2" s="2" t="s">
+        <v>168</v>
+      </c>
+    </row>
+    <row r="3" spans="2:4" ht="37.5" x14ac:dyDescent="0.25">
       <c r="B3" s="13" t="s">
         <v>95</v>
       </c>
       <c r="C3" s="5" t="s">
         <v>144</v>
       </c>
-    </row>
-    <row r="4" spans="2:3" ht="18.75" x14ac:dyDescent="0.25">
+      <c r="D3" s="8" t="s">
+        <v>115</v>
+      </c>
+    </row>
+    <row r="4" spans="2:4" ht="18.75" x14ac:dyDescent="0.25">
       <c r="B4" s="14" t="s">
         <v>117</v>
       </c>
       <c r="C4" s="8" t="s">
         <v>115</v>
       </c>
-    </row>
-    <row r="5" spans="2:3" ht="18.75" x14ac:dyDescent="0.25">
+      <c r="D4" s="8" t="s">
+        <v>115</v>
+      </c>
+    </row>
+    <row r="5" spans="2:4" ht="18.75" x14ac:dyDescent="0.25">
       <c r="B5" s="14" t="s">
         <v>118</v>
       </c>
       <c r="C5" s="8" t="s">
         <v>115</v>
       </c>
-    </row>
-    <row r="6" spans="2:3" ht="18.75" x14ac:dyDescent="0.25">
+      <c r="D5" s="8" t="s">
+        <v>115</v>
+      </c>
+    </row>
+    <row r="6" spans="2:4" ht="18.75" x14ac:dyDescent="0.25">
       <c r="B6" s="14" t="s">
         <v>119</v>
       </c>
       <c r="C6" s="8" t="s">
         <v>115</v>
       </c>
-    </row>
-    <row r="7" spans="2:3" ht="18.75" x14ac:dyDescent="0.25">
+      <c r="D6" s="8" t="s">
+        <v>115</v>
+      </c>
+    </row>
+    <row r="7" spans="2:4" ht="18.75" x14ac:dyDescent="0.25">
       <c r="B7" s="14" t="s">
         <v>120</v>
       </c>
       <c r="C7" s="8" t="s">
         <v>115</v>
       </c>
-    </row>
-    <row r="8" spans="2:3" ht="18.75" x14ac:dyDescent="0.25">
+      <c r="D7" s="8" t="s">
+        <v>115</v>
+      </c>
+    </row>
+    <row r="8" spans="2:4" ht="18.75" x14ac:dyDescent="0.25">
       <c r="B8" s="14" t="s">
         <v>121</v>
       </c>
       <c r="C8" s="8" t="s">
         <v>115</v>
       </c>
-    </row>
-    <row r="9" spans="2:3" ht="37.5" x14ac:dyDescent="0.25">
+      <c r="D8" s="8" t="s">
+        <v>115</v>
+      </c>
+    </row>
+    <row r="9" spans="2:4" ht="37.5" x14ac:dyDescent="0.25">
       <c r="B9" s="14" t="s">
         <v>122</v>
       </c>
       <c r="C9" s="8" t="s">
         <v>144</v>
       </c>
-    </row>
-    <row r="10" spans="2:3" ht="75" x14ac:dyDescent="0.25">
+      <c r="D9" s="8" t="s">
+        <v>115</v>
+      </c>
+    </row>
+    <row r="10" spans="2:4" ht="75" x14ac:dyDescent="0.25">
       <c r="B10" s="14" t="s">
         <v>123</v>
       </c>
       <c r="C10" s="8" t="s">
-        <v>145</v>
-      </c>
-    </row>
-    <row r="11" spans="2:3" ht="37.5" x14ac:dyDescent="0.25">
+        <v>177</v>
+      </c>
+      <c r="D10" s="8" t="s">
+        <v>115</v>
+      </c>
+    </row>
+    <row r="11" spans="2:4" ht="37.5" x14ac:dyDescent="0.25">
       <c r="B11" s="14" t="s">
         <v>124</v>
       </c>
       <c r="C11" s="8" t="s">
         <v>144</v>
       </c>
-    </row>
-    <row r="12" spans="2:3" ht="18.75" hidden="1" x14ac:dyDescent="0.25">
+      <c r="D11" s="8" t="s">
+        <v>115</v>
+      </c>
+    </row>
+    <row r="12" spans="2:4" ht="18.75" hidden="1" x14ac:dyDescent="0.25">
       <c r="B12" s="14"/>
       <c r="C12" s="8"/>
-    </row>
-    <row r="13" spans="2:3" ht="18.75" x14ac:dyDescent="0.25">
+      <c r="D12" s="8"/>
+    </row>
+    <row r="13" spans="2:4" ht="18.75" x14ac:dyDescent="0.25">
       <c r="B13" s="14" t="s">
         <v>113</v>
       </c>
       <c r="C13" s="8" t="s">
         <v>115</v>
       </c>
-    </row>
-    <row r="14" spans="2:3" ht="18.75" x14ac:dyDescent="0.25">
+      <c r="D13" s="8" t="s">
+        <v>115</v>
+      </c>
+    </row>
+    <row r="14" spans="2:4" ht="18.75" x14ac:dyDescent="0.25">
       <c r="B14" s="14" t="s">
         <v>114</v>
       </c>
       <c r="C14" s="8" t="s">
         <v>115</v>
       </c>
-    </row>
-    <row r="15" spans="2:3" ht="93.75" x14ac:dyDescent="0.25">
+      <c r="D14" s="8" t="s">
+        <v>115</v>
+      </c>
+    </row>
+    <row r="15" spans="2:4" ht="93.75" x14ac:dyDescent="0.25">
       <c r="B15" s="14" t="s">
         <v>125</v>
       </c>
       <c r="C15" s="8" t="s">
-        <v>146</v>
-      </c>
-    </row>
-    <row r="16" spans="2:3" ht="18.75" x14ac:dyDescent="0.25">
+        <v>145</v>
+      </c>
+      <c r="D15" s="8" t="s">
+        <v>115</v>
+      </c>
+    </row>
+    <row r="16" spans="2:4" ht="18.75" x14ac:dyDescent="0.25">
       <c r="B16" s="14" t="s">
         <v>126</v>
       </c>
       <c r="C16" s="8" t="s">
         <v>115</v>
       </c>
-    </row>
-    <row r="17" spans="2:3" ht="18.75" x14ac:dyDescent="0.25">
+      <c r="D16" s="8" t="s">
+        <v>115</v>
+      </c>
+    </row>
+    <row r="17" spans="2:4" ht="18.75" x14ac:dyDescent="0.25">
       <c r="B17" s="14" t="s">
         <v>127</v>
       </c>
       <c r="C17" s="8" t="s">
         <v>115</v>
       </c>
-    </row>
-    <row r="18" spans="2:3" ht="18.75" x14ac:dyDescent="0.25">
+      <c r="D17" s="8" t="s">
+        <v>115</v>
+      </c>
+    </row>
+    <row r="18" spans="2:4" ht="18.75" x14ac:dyDescent="0.25">
       <c r="B18" s="14" t="s">
         <v>128</v>
       </c>
       <c r="C18" s="8" t="s">
+        <v>115</v>
+      </c>
+      <c r="D18" s="8" t="s">
         <v>115</v>
       </c>
     </row>
@@ -5978,176 +6190,237 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2D00C403-3C77-4C50-8FD7-B532FB244FE1}">
-  <dimension ref="B1:C21"/>
+  <dimension ref="B1:D21"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B2" sqref="B2:C10"/>
+      <selection activeCell="D8" sqref="D8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="2" max="2" width="26" customWidth="1"/>
     <col min="3" max="3" width="23.140625" customWidth="1"/>
+    <col min="4" max="4" width="24.140625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="2:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
-    <row r="2" spans="2:3" ht="47.25" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="1" spans="2:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
+    <row r="2" spans="2:4" ht="70.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B2" s="2" t="s">
         <v>94</v>
       </c>
       <c r="C2" s="2" t="s">
         <v>43</v>
       </c>
-    </row>
-    <row r="3" spans="2:3" ht="56.25" x14ac:dyDescent="0.25">
+      <c r="D2" s="2" t="s">
+        <v>168</v>
+      </c>
+    </row>
+    <row r="3" spans="2:4" ht="56.25" x14ac:dyDescent="0.25">
       <c r="B3" s="13" t="s">
         <v>95</v>
       </c>
       <c r="C3" s="5" t="s">
         <v>143</v>
       </c>
-    </row>
-    <row r="4" spans="2:3" ht="18.75" x14ac:dyDescent="0.25">
+      <c r="D3" s="8" t="s">
+        <v>115</v>
+      </c>
+    </row>
+    <row r="4" spans="2:4" ht="18.75" x14ac:dyDescent="0.25">
       <c r="B4" s="14" t="s">
         <v>129</v>
       </c>
       <c r="C4" s="8" t="s">
         <v>115</v>
       </c>
-    </row>
-    <row r="5" spans="2:3" ht="18.75" x14ac:dyDescent="0.25">
+      <c r="D4" s="8" t="s">
+        <v>115</v>
+      </c>
+    </row>
+    <row r="5" spans="2:4" ht="18.75" x14ac:dyDescent="0.25">
       <c r="B5" s="14" t="s">
         <v>130</v>
       </c>
       <c r="C5" s="8" t="s">
         <v>115</v>
       </c>
-    </row>
-    <row r="6" spans="2:3" ht="18.75" x14ac:dyDescent="0.25">
+      <c r="D5" s="8" t="s">
+        <v>115</v>
+      </c>
+    </row>
+    <row r="6" spans="2:4" ht="18.75" x14ac:dyDescent="0.25">
       <c r="B6" s="14" t="s">
         <v>131</v>
       </c>
       <c r="C6" s="8" t="s">
         <v>115</v>
       </c>
-    </row>
-    <row r="7" spans="2:3" ht="18.75" x14ac:dyDescent="0.25">
+      <c r="D6" s="8" t="s">
+        <v>115</v>
+      </c>
+    </row>
+    <row r="7" spans="2:4" ht="18.75" x14ac:dyDescent="0.25">
       <c r="B7" s="14" t="s">
         <v>132</v>
       </c>
       <c r="C7" s="8" t="s">
         <v>115</v>
       </c>
-    </row>
-    <row r="8" spans="2:3" ht="18.75" x14ac:dyDescent="0.25">
+      <c r="D7" s="8" t="s">
+        <v>115</v>
+      </c>
+    </row>
+    <row r="8" spans="2:4" ht="150" x14ac:dyDescent="0.25">
       <c r="B8" s="14" t="s">
         <v>133</v>
       </c>
       <c r="C8" s="8" t="s">
         <v>115</v>
       </c>
-    </row>
-    <row r="9" spans="2:3" ht="18.75" x14ac:dyDescent="0.25">
+      <c r="D8" s="8" t="s">
+        <v>172</v>
+      </c>
+    </row>
+    <row r="9" spans="2:4" ht="150" x14ac:dyDescent="0.25">
       <c r="B9" s="14" t="s">
         <v>134</v>
       </c>
       <c r="C9" s="8" t="s">
         <v>115</v>
       </c>
-    </row>
-    <row r="10" spans="2:3" ht="18.75" x14ac:dyDescent="0.25">
+      <c r="D9" s="8" t="s">
+        <v>172</v>
+      </c>
+    </row>
+    <row r="10" spans="2:4" ht="75" x14ac:dyDescent="0.25">
       <c r="B10" s="14" t="s">
         <v>135</v>
       </c>
       <c r="C10" s="8" t="s">
         <v>115</v>
       </c>
-    </row>
-    <row r="11" spans="2:3" ht="18.75" x14ac:dyDescent="0.25">
+      <c r="D10" s="8" t="s">
+        <v>173</v>
+      </c>
+    </row>
+    <row r="11" spans="2:4" ht="18.75" x14ac:dyDescent="0.25">
       <c r="B11" s="14" t="s">
         <v>136</v>
       </c>
       <c r="C11" s="8" t="s">
         <v>115</v>
       </c>
-    </row>
-    <row r="12" spans="2:3" ht="18.75" x14ac:dyDescent="0.25">
+      <c r="D11" s="8" t="s">
+        <v>115</v>
+      </c>
+    </row>
+    <row r="12" spans="2:4" ht="18.75" x14ac:dyDescent="0.25">
       <c r="B12" s="14" t="s">
         <v>117</v>
       </c>
       <c r="C12" s="8" t="s">
         <v>115</v>
       </c>
-    </row>
-    <row r="13" spans="2:3" ht="18.75" x14ac:dyDescent="0.25">
+      <c r="D12" s="8" t="s">
+        <v>115</v>
+      </c>
+    </row>
+    <row r="13" spans="2:4" ht="37.5" x14ac:dyDescent="0.25">
       <c r="B13" s="14" t="s">
         <v>137</v>
       </c>
       <c r="C13" s="8" t="s">
         <v>115</v>
       </c>
-    </row>
-    <row r="14" spans="2:3" ht="18.75" x14ac:dyDescent="0.25">
+      <c r="D13" s="8" t="s">
+        <v>171</v>
+      </c>
+    </row>
+    <row r="14" spans="2:4" ht="18.75" x14ac:dyDescent="0.25">
       <c r="B14" s="14" t="s">
         <v>138</v>
       </c>
       <c r="C14" s="8" t="s">
         <v>115</v>
       </c>
-    </row>
-    <row r="15" spans="2:3" ht="18.75" x14ac:dyDescent="0.25">
+      <c r="D14" s="8" t="s">
+        <v>115</v>
+      </c>
+    </row>
+    <row r="15" spans="2:4" ht="18.75" x14ac:dyDescent="0.25">
       <c r="B15" s="14" t="s">
         <v>139</v>
       </c>
       <c r="C15" s="8" t="s">
         <v>115</v>
       </c>
-    </row>
-    <row r="16" spans="2:3" ht="18.75" x14ac:dyDescent="0.25">
+      <c r="D15" s="8" t="s">
+        <v>115</v>
+      </c>
+    </row>
+    <row r="16" spans="2:4" ht="112.5" x14ac:dyDescent="0.25">
       <c r="B16" s="14" t="s">
         <v>140</v>
       </c>
       <c r="C16" s="8" t="s">
         <v>115</v>
       </c>
-    </row>
-    <row r="17" spans="2:3" ht="18.75" x14ac:dyDescent="0.25">
+      <c r="D16" s="8" t="s">
+        <v>174</v>
+      </c>
+    </row>
+    <row r="17" spans="2:4" ht="112.5" x14ac:dyDescent="0.25">
       <c r="B17" s="14" t="s">
         <v>141</v>
       </c>
       <c r="C17" s="8" t="s">
         <v>115</v>
       </c>
-    </row>
-    <row r="18" spans="2:3" ht="18.75" x14ac:dyDescent="0.25">
+      <c r="D17" s="8" t="s">
+        <v>174</v>
+      </c>
+    </row>
+    <row r="18" spans="2:4" ht="18.75" x14ac:dyDescent="0.25">
       <c r="B18" s="14" t="s">
         <v>142</v>
       </c>
       <c r="C18" s="8" t="s">
         <v>115</v>
       </c>
-    </row>
-    <row r="19" spans="2:3" ht="18.75" x14ac:dyDescent="0.25">
+      <c r="D18" s="8" t="s">
+        <v>115</v>
+      </c>
+    </row>
+    <row r="19" spans="2:4" ht="18.75" x14ac:dyDescent="0.25">
       <c r="B19" s="14" t="s">
         <v>114</v>
       </c>
       <c r="C19" s="8" t="s">
         <v>115</v>
       </c>
-    </row>
-    <row r="20" spans="2:3" ht="18.75" x14ac:dyDescent="0.25">
+      <c r="D19" s="8" t="s">
+        <v>115</v>
+      </c>
+    </row>
+    <row r="20" spans="2:4" ht="112.5" x14ac:dyDescent="0.25">
       <c r="B20" s="14" t="s">
         <v>112</v>
       </c>
       <c r="C20" s="8" t="s">
         <v>115</v>
       </c>
-    </row>
-    <row r="21" spans="2:3" ht="18.75" x14ac:dyDescent="0.25">
+      <c r="D20" s="8" t="s">
+        <v>174</v>
+      </c>
+    </row>
+    <row r="21" spans="2:4" ht="18.75" x14ac:dyDescent="0.25">
       <c r="B21" s="14" t="s">
         <v>113</v>
       </c>
       <c r="C21" s="8" t="s">
+        <v>115</v>
+      </c>
+      <c r="D21" s="8" t="s">
         <v>115</v>
       </c>
     </row>
@@ -6158,88 +6431,116 @@
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{DCA707A4-84AD-4A37-9A2B-76628AC8689E}">
-  <dimension ref="B1:C10"/>
+  <dimension ref="B1:D10"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C10" sqref="C10"/>
+      <selection activeCell="H6" sqref="H6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="2" max="2" width="32.85546875" customWidth="1"/>
     <col min="3" max="3" width="23.140625" customWidth="1"/>
+    <col min="4" max="4" width="23.7109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="2:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
-    <row r="2" spans="2:3" ht="47.25" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="1" spans="2:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
+    <row r="2" spans="2:4" ht="93.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B2" s="2" t="s">
         <v>94</v>
       </c>
       <c r="C2" s="2" t="s">
         <v>43</v>
       </c>
-    </row>
-    <row r="3" spans="2:3" ht="56.25" x14ac:dyDescent="0.25">
+      <c r="D2" s="2" t="s">
+        <v>168</v>
+      </c>
+    </row>
+    <row r="3" spans="2:4" ht="131.25" x14ac:dyDescent="0.25">
       <c r="B3" s="13" t="s">
         <v>95</v>
       </c>
       <c r="C3" s="5" t="s">
-        <v>155</v>
-      </c>
-    </row>
-    <row r="4" spans="2:3" ht="18.75" x14ac:dyDescent="0.25">
+        <v>176</v>
+      </c>
+      <c r="D3" s="8" t="s">
+        <v>181</v>
+      </c>
+    </row>
+    <row r="4" spans="2:4" ht="37.5" x14ac:dyDescent="0.25">
       <c r="B4" s="14" t="s">
+        <v>146</v>
+      </c>
+      <c r="C4" s="8" t="s">
+        <v>115</v>
+      </c>
+      <c r="D4" s="8" t="s">
+        <v>115</v>
+      </c>
+    </row>
+    <row r="5" spans="2:4" ht="131.25" x14ac:dyDescent="0.25">
+      <c r="B5" s="14" t="s">
+        <v>147</v>
+      </c>
+      <c r="C5" s="5" t="s">
+        <v>176</v>
+      </c>
+      <c r="D5" s="8" t="s">
+        <v>181</v>
+      </c>
+    </row>
+    <row r="6" spans="2:4" ht="131.25" x14ac:dyDescent="0.25">
+      <c r="B6" s="14" t="s">
         <v>148</v>
       </c>
-      <c r="C4" s="8" t="s">
-        <v>115</v>
-      </c>
-    </row>
-    <row r="5" spans="2:3" ht="56.25" x14ac:dyDescent="0.25">
-      <c r="B5" s="14" t="s">
+      <c r="C6" s="5" t="s">
+        <v>176</v>
+      </c>
+      <c r="D6" s="8" t="s">
+        <v>181</v>
+      </c>
+    </row>
+    <row r="7" spans="2:4" ht="131.25" x14ac:dyDescent="0.25">
+      <c r="B7" s="14" t="s">
         <v>149</v>
       </c>
-      <c r="C5" s="8" t="s">
-        <v>155</v>
-      </c>
-    </row>
-    <row r="6" spans="2:3" ht="56.25" x14ac:dyDescent="0.25">
-      <c r="B6" s="14" t="s">
+      <c r="C7" s="5" t="s">
+        <v>176</v>
+      </c>
+      <c r="D7" s="8" t="s">
+        <v>181</v>
+      </c>
+    </row>
+    <row r="8" spans="2:4" ht="56.25" x14ac:dyDescent="0.25">
+      <c r="B8" s="14" t="s">
         <v>150</v>
       </c>
-      <c r="C6" s="8" t="s">
-        <v>155</v>
-      </c>
-    </row>
-    <row r="7" spans="2:3" ht="56.25" x14ac:dyDescent="0.25">
-      <c r="B7" s="14" t="s">
+      <c r="C8" s="5" t="s">
+        <v>176</v>
+      </c>
+      <c r="D8" s="8" t="s">
+        <v>180</v>
+      </c>
+    </row>
+    <row r="9" spans="2:4" ht="56.25" x14ac:dyDescent="0.25">
+      <c r="B9" s="14" t="s">
         <v>151</v>
       </c>
-      <c r="C7" s="8" t="s">
-        <v>155</v>
-      </c>
-    </row>
-    <row r="8" spans="2:3" ht="56.25" x14ac:dyDescent="0.25">
-      <c r="B8" s="14" t="s">
+      <c r="C9" s="5" t="s">
+        <v>176</v>
+      </c>
+      <c r="D9" s="8" t="s">
+        <v>175</v>
+      </c>
+    </row>
+    <row r="10" spans="2:4" ht="37.5" x14ac:dyDescent="0.25">
+      <c r="B10" s="14" t="s">
         <v>152</v>
       </c>
-      <c r="C8" s="8" t="s">
-        <v>155</v>
-      </c>
-    </row>
-    <row r="9" spans="2:3" ht="56.25" x14ac:dyDescent="0.25">
-      <c r="B9" s="14" t="s">
-        <v>153</v>
-      </c>
-      <c r="C9" s="8" t="s">
-        <v>155</v>
-      </c>
-    </row>
-    <row r="10" spans="2:3" ht="18.75" x14ac:dyDescent="0.25">
-      <c r="B10" s="14" t="s">
-        <v>154</v>
-      </c>
       <c r="C10" s="8" t="s">
+        <v>115</v>
+      </c>
+      <c r="D10" s="8" t="s">
         <v>115</v>
       </c>
     </row>
@@ -6250,65 +6551,95 @@
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{19264B5D-9C82-4108-AEE9-967C34FA97B5}">
-  <dimension ref="B1:C7"/>
+  <dimension ref="B1:D8"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C3" sqref="C3"/>
+      <selection activeCell="D2" sqref="D2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="2" max="2" width="23.5703125" customWidth="1"/>
     <col min="3" max="3" width="22.28515625" customWidth="1"/>
+    <col min="4" max="4" width="23.85546875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="2:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
-    <row r="2" spans="2:3" ht="47.25" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="1" spans="2:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
+    <row r="2" spans="2:4" ht="93.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B2" s="2" t="s">
         <v>94</v>
       </c>
       <c r="C2" s="2" t="s">
         <v>43</v>
       </c>
-    </row>
-    <row r="3" spans="2:3" ht="56.25" x14ac:dyDescent="0.25">
+      <c r="D2" s="2" t="s">
+        <v>168</v>
+      </c>
+    </row>
+    <row r="3" spans="2:4" ht="131.25" x14ac:dyDescent="0.25">
       <c r="B3" s="13" t="s">
         <v>95</v>
       </c>
       <c r="C3" s="5" t="s">
+        <v>153</v>
+      </c>
+      <c r="D3" s="8" t="s">
+        <v>181</v>
+      </c>
+    </row>
+    <row r="4" spans="2:4" ht="131.25" x14ac:dyDescent="0.25">
+      <c r="B4" s="14" t="s">
+        <v>156</v>
+      </c>
+      <c r="C4" s="8" t="s">
+        <v>153</v>
+      </c>
+      <c r="D4" s="8" t="s">
+        <v>181</v>
+      </c>
+    </row>
+    <row r="5" spans="2:4" ht="131.25" x14ac:dyDescent="0.25">
+      <c r="B5" s="14" t="s">
         <v>155</v>
       </c>
-    </row>
-    <row r="4" spans="2:3" ht="56.25" x14ac:dyDescent="0.25">
-      <c r="B4" s="14" t="s">
-        <v>158</v>
-      </c>
-      <c r="C4" s="8" t="s">
-        <v>155</v>
-      </c>
-    </row>
-    <row r="5" spans="2:3" ht="56.25" x14ac:dyDescent="0.25">
-      <c r="B5" s="14" t="s">
-        <v>157</v>
-      </c>
       <c r="C5" s="8" t="s">
-        <v>155</v>
-      </c>
-    </row>
-    <row r="6" spans="2:3" ht="56.25" x14ac:dyDescent="0.25">
+        <v>153</v>
+      </c>
+      <c r="D5" s="8" t="s">
+        <v>181</v>
+      </c>
+    </row>
+    <row r="6" spans="2:4" ht="131.25" x14ac:dyDescent="0.25">
       <c r="B6" s="14" t="s">
-        <v>156</v>
+        <v>154</v>
       </c>
       <c r="C6" s="8" t="s">
-        <v>155</v>
-      </c>
-    </row>
-    <row r="7" spans="2:3" ht="56.25" x14ac:dyDescent="0.25">
+        <v>153</v>
+      </c>
+      <c r="D6" s="8" t="s">
+        <v>181</v>
+      </c>
+    </row>
+    <row r="7" spans="2:4" ht="131.25" x14ac:dyDescent="0.25">
       <c r="B7" s="14" t="s">
         <v>113</v>
       </c>
       <c r="C7" s="8" t="s">
-        <v>155</v>
+        <v>153</v>
+      </c>
+      <c r="D7" s="8" t="s">
+        <v>181</v>
+      </c>
+    </row>
+    <row r="8" spans="2:4" ht="18.75" x14ac:dyDescent="0.25">
+      <c r="B8" s="14" t="s">
+        <v>126</v>
+      </c>
+      <c r="C8" s="8" t="s">
+        <v>115</v>
+      </c>
+      <c r="D8" s="8" t="s">
+        <v>115</v>
       </c>
     </row>
   </sheetData>
@@ -6318,128 +6649,171 @@
 
 <file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0107F7F4-65A4-4F3B-ABD6-BF0903CF1797}">
-  <dimension ref="B1:C15"/>
+  <dimension ref="B1:D15"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D12" sqref="D12"/>
+      <selection activeCell="E2" sqref="E2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="2" max="2" width="28.5703125" customWidth="1"/>
     <col min="3" max="3" width="22.7109375" customWidth="1"/>
+    <col min="4" max="4" width="24" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="2:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
-    <row r="2" spans="2:3" ht="47.25" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="1" spans="2:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
+    <row r="2" spans="2:4" ht="47.25" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B2" s="2" t="s">
         <v>94</v>
       </c>
       <c r="C2" s="2" t="s">
         <v>43</v>
       </c>
-    </row>
-    <row r="3" spans="2:3" ht="18.75" x14ac:dyDescent="0.25">
+      <c r="D2" s="2" t="s">
+        <v>168</v>
+      </c>
+    </row>
+    <row r="3" spans="2:4" ht="300" x14ac:dyDescent="0.25">
       <c r="B3" s="13" t="s">
         <v>95</v>
       </c>
       <c r="C3" s="8" t="s">
         <v>115</v>
       </c>
-    </row>
-    <row r="4" spans="2:3" ht="18.75" x14ac:dyDescent="0.25">
+      <c r="D3" s="8" t="s">
+        <v>182</v>
+      </c>
+    </row>
+    <row r="4" spans="2:4" ht="300" x14ac:dyDescent="0.25">
       <c r="B4" s="14" t="s">
+        <v>157</v>
+      </c>
+      <c r="C4" s="8" t="s">
+        <v>115</v>
+      </c>
+      <c r="D4" s="8" t="s">
+        <v>182</v>
+      </c>
+    </row>
+    <row r="5" spans="2:4" ht="300" x14ac:dyDescent="0.25">
+      <c r="B5" s="14" t="s">
+        <v>158</v>
+      </c>
+      <c r="C5" s="8" t="s">
+        <v>115</v>
+      </c>
+      <c r="D5" s="8" t="s">
+        <v>182</v>
+      </c>
+    </row>
+    <row r="6" spans="2:4" ht="300" x14ac:dyDescent="0.25">
+      <c r="B6" s="14" t="s">
         <v>159</v>
       </c>
-      <c r="C4" s="8" t="s">
-        <v>115</v>
-      </c>
-    </row>
-    <row r="5" spans="2:3" ht="18.75" x14ac:dyDescent="0.25">
-      <c r="B5" s="14" t="s">
+      <c r="C6" s="8" t="s">
+        <v>115</v>
+      </c>
+      <c r="D6" s="8" t="s">
+        <v>182</v>
+      </c>
+    </row>
+    <row r="7" spans="2:4" ht="300" x14ac:dyDescent="0.25">
+      <c r="B7" s="14" t="s">
         <v>160</v>
       </c>
-      <c r="C5" s="8" t="s">
-        <v>115</v>
-      </c>
-    </row>
-    <row r="6" spans="2:3" ht="18.75" x14ac:dyDescent="0.25">
-      <c r="B6" s="14" t="s">
+      <c r="C7" s="8" t="s">
+        <v>115</v>
+      </c>
+      <c r="D7" s="8" t="s">
+        <v>182</v>
+      </c>
+    </row>
+    <row r="8" spans="2:4" ht="300" x14ac:dyDescent="0.25">
+      <c r="B8" s="14" t="s">
         <v>161</v>
       </c>
-      <c r="C6" s="8" t="s">
-        <v>115</v>
-      </c>
-    </row>
-    <row r="7" spans="2:3" ht="18.75" x14ac:dyDescent="0.25">
-      <c r="B7" s="14" t="s">
+      <c r="C8" s="8" t="s">
+        <v>115</v>
+      </c>
+      <c r="D8" s="8" t="s">
+        <v>182</v>
+      </c>
+    </row>
+    <row r="9" spans="2:4" ht="300" x14ac:dyDescent="0.25">
+      <c r="B9" s="14" t="s">
         <v>162</v>
       </c>
-      <c r="C7" s="8" t="s">
-        <v>115</v>
-      </c>
-    </row>
-    <row r="8" spans="2:3" ht="18.75" x14ac:dyDescent="0.25">
-      <c r="B8" s="14" t="s">
+      <c r="C9" s="8" t="s">
+        <v>115</v>
+      </c>
+      <c r="D9" s="8" t="s">
+        <v>182</v>
+      </c>
+    </row>
+    <row r="10" spans="2:4" ht="300" x14ac:dyDescent="0.25">
+      <c r="B10" s="14" t="s">
         <v>163</v>
       </c>
-      <c r="C8" s="8" t="s">
-        <v>115</v>
-      </c>
-    </row>
-    <row r="9" spans="2:3" ht="18.75" x14ac:dyDescent="0.25">
-      <c r="B9" s="14" t="s">
+      <c r="C10" s="8" t="s">
+        <v>115</v>
+      </c>
+      <c r="D10" s="8" t="s">
+        <v>182</v>
+      </c>
+    </row>
+    <row r="11" spans="2:4" ht="300" x14ac:dyDescent="0.25">
+      <c r="B11" s="14" t="s">
         <v>164</v>
       </c>
-      <c r="C9" s="8" t="s">
-        <v>115</v>
-      </c>
-    </row>
-    <row r="10" spans="2:3" ht="37.5" x14ac:dyDescent="0.25">
-      <c r="B10" s="14" t="s">
+      <c r="C11" s="8" t="s">
+        <v>115</v>
+      </c>
+      <c r="D11" s="8" t="s">
+        <v>182</v>
+      </c>
+    </row>
+    <row r="12" spans="2:4" ht="300" x14ac:dyDescent="0.25">
+      <c r="B12" s="14" t="s">
         <v>165</v>
       </c>
-      <c r="C10" s="8" t="s">
-        <v>115</v>
-      </c>
-    </row>
-    <row r="11" spans="2:3" ht="37.5" x14ac:dyDescent="0.25">
-      <c r="B11" s="14" t="s">
+      <c r="C12" s="8" t="s">
+        <v>115</v>
+      </c>
+      <c r="D12" s="8" t="s">
+        <v>182</v>
+      </c>
+    </row>
+    <row r="13" spans="2:4" ht="300" x14ac:dyDescent="0.25">
+      <c r="B13" s="14" t="s">
         <v>166</v>
       </c>
-      <c r="C11" s="8" t="s">
-        <v>115</v>
-      </c>
-    </row>
-    <row r="12" spans="2:3" ht="37.5" x14ac:dyDescent="0.25">
-      <c r="B12" s="14" t="s">
+      <c r="C13" s="8" t="s">
+        <v>115</v>
+      </c>
+      <c r="D13" s="8" t="s">
+        <v>182</v>
+      </c>
+    </row>
+    <row r="14" spans="2:4" ht="300" x14ac:dyDescent="0.25">
+      <c r="B14" s="14" t="s">
         <v>167</v>
       </c>
-      <c r="C12" s="8" t="s">
-        <v>115</v>
-      </c>
-    </row>
-    <row r="13" spans="2:3" ht="37.5" x14ac:dyDescent="0.25">
-      <c r="B13" s="14" t="s">
-        <v>168</v>
-      </c>
-      <c r="C13" s="8" t="s">
-        <v>115</v>
-      </c>
-    </row>
-    <row r="14" spans="2:3" ht="37.5" x14ac:dyDescent="0.25">
-      <c r="B14" s="14" t="s">
-        <v>169</v>
-      </c>
       <c r="C14" s="8" t="s">
         <v>115</v>
       </c>
-    </row>
-    <row r="15" spans="2:3" ht="18.75" x14ac:dyDescent="0.25">
+      <c r="D14" s="8" t="s">
+        <v>182</v>
+      </c>
+    </row>
+    <row r="15" spans="2:4" ht="37.5" x14ac:dyDescent="0.25">
       <c r="B15" s="14" t="s">
         <v>112</v>
       </c>
       <c r="C15" s="8" t="s">
+        <v>115</v>
+      </c>
+      <c r="D15" s="8" t="s">
         <v>115</v>
       </c>
     </row>

</xml_diff>